<commit_message>
changing the name of a sheet
</commit_message>
<xml_diff>
--- a/exercises/03-collaborative-enterprise-planning/datasets/maintenance-cost-master-data.xlsx
+++ b/exercises/03-collaborative-enterprise-planning/datasets/maintenance-cost-master-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/dayanand_karalkar_sap_com/Documents/D2V Exercises Master Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/cesare_calabria_sap_com/Documents/Documents/D2V2.0_PREP/riusciremo_mai/btp-ai-sustainability-bootcamp/exercises/03-collaborative-enterprise-planning/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{2A6AF761-4022-4BEE-AAD0-7C89BD0B22E8}" xr6:coauthVersionLast="48" xr6:coauthVersionMax="48" xr10:uidLastSave="{D6B491CA-7D73-45D4-A965-24ECF2832F21}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{2A6AF761-4022-4BEE-AAD0-7C89BD0B22E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{0C2AFB6A-9B41-B541-8514-45CEA9B4C5D7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="5" activeTab="4" xr2:uid="{12130E0B-80C8-4F75-B685-2989B6CFCA33}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33340" windowHeight="21580" activeTab="5" xr2:uid="{12130E0B-80C8-4F75-B685-2989B6CFCA33}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Company Code" sheetId="3" r:id="rId3"/>
     <sheet name="Cost Center" sheetId="4" r:id="rId4"/>
     <sheet name="Plant" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
+    <sheet name="Maintenance Category" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028" concurrentManualCount="8"/>
   <extLst>
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,14 +484,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>220300010</v>
       </c>
@@ -513,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>220300020</v>
       </c>
@@ -524,7 +524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>220300031</v>
       </c>
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>220300032</v>
       </c>
@@ -546,7 +546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>220300033</v>
       </c>
@@ -557,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>220300034</v>
       </c>
@@ -568,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>220300035</v>
       </c>
@@ -579,7 +579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>220300036</v>
       </c>
@@ -607,13 +607,13 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -635,7 +635,7 @@
         <v>10101301</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -646,7 +646,7 @@
         <v>10101301</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -674,12 +674,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1010</v>
       </c>
@@ -717,12 +717,12 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10101301</v>
       </c>
@@ -750,16 +750,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B6C860-E8DA-44BD-8091-8EAC41D7633F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1010</v>
       </c>
@@ -787,16 +787,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D879E9-C63D-440C-9F9F-76320EDB94BB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -804,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -812,7 +812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -820,7 +820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -837,6 +837,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000F194946EA0D147A884CDD59C7E0164" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6f1930fb59ca44fc25c09677fd00d5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="54f01c01-2f85-4966-a6d1-afec7cd337eb" xmlns:ns3="0f6111bb-91e8-4312-abe0-71d36b36fa1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d0d682b63acdf024d13ce4199759422" ns2:_="" ns3:_="">
     <xsd:import namespace="54f01c01-2f85-4966-a6d1-afec7cd337eb"/>
@@ -1053,29 +1068,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E9B821A-5C13-4CC9-890A-CBE4E56220FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ECD1946-CD42-467F-9048-97E48C8D4F70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="54f01c01-2f85-4966-a6d1-afec7cd337eb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0f6111bb-91e8-4312-abe0-71d36b36fa1f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{871E2B4A-580D-4F5D-8C75-8B7F895E8143}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{871E2B4A-580D-4F5D-8C75-8B7F895E8143}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ECD1946-CD42-467F-9048-97E48C8D4F70}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E9B821A-5C13-4CC9-890A-CBE4E56220FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="54f01c01-2f85-4966-a6d1-afec7cd337eb"/>
+    <ds:schemaRef ds:uri="0f6111bb-91e8-4312-abe0-71d36b36fa1f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>